<commit_message>
Updated R scripts to use new DCT
</commit_message>
<xml_diff>
--- a/WISNInputs.xlsx
+++ b/WISNInputs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Mwasi/Palladium/DataFi-HRH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEBB831-EAD0-D043-B2B7-F5DEAB2643AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA46011-FDA0-9144-BFC3-C2D0E2B87D71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15640" xr2:uid="{59FBE346-4569-2A48-8E6D-CBB363BFD9B4}"/>
+    <workbookView xWindow="1180" yWindow="1440" windowWidth="27240" windowHeight="15640" activeTab="1" xr2:uid="{59FBE346-4569-2A48-8E6D-CBB363BFD9B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Client Time" sheetId="1" r:id="rId1"/>
+    <sheet name="Program Area" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="20">
   <si>
     <t>Cadre</t>
   </si>
@@ -90,6 +91,9 @@
   </si>
   <si>
     <t>ClientTime</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -125,8 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -153,6 +160,17 @@
     <tableColumn id="3" xr3:uid="{8AED856E-A0EE-354C-B40B-D5B691C131C4}" name="ClientTime"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF221680-F6B2-EA41-A656-559B7A4D08A3}" name="Table2" displayName="Table2" ref="A1:B9" totalsRowShown="0">
+  <autoFilter ref="A1:B9" xr:uid="{A27919D9-8068-B84A-B3EB-7B4239061F1F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{3EFAE52B-704E-FB45-9B53-34CC9AA52AA2}" name="ProgramArea"/>
+    <tableColumn id="2" xr3:uid="{08503BDD-69A2-EE46-AA16-60F83A61D69E}" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -455,7 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358D9F6A-7699-5C49-A3F2-187D6D2429EC}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1187,4 +1205,74 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D6145A-48AA-AD45-BB58-184586778D21}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>